<commit_message>
Final version of some reports and RTL Freeze checklist.
Signed-off-by: Pascal Gouedo <pascal.gouedo@dolphin.fr>
</commit_message>
<xml_diff>
--- a/Project-Descriptions-and-Plans/CV32E40Pv2/Milestone-data/RTL_v1.8.3/CV32E40Pv2_not_verified_features.xlsx
+++ b/Project-Descriptions-and-Plans/CV32E40Pv2/Milestone-data/RTL_v1.8.3/CV32E40Pv2_not_verified_features.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\git_repos\programs\programs\Project-Descriptions-and-Plans\CV32E40Pv2\Milestone-data\RTL_v1.8.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\core-v-docs\Project-Descriptions-and-Plans\CV32E40Pv2\Milestone-data\RTL_v1.8.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC83A268-E424-40B9-B91E-882922428600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1844F7-72AD-4BF7-A381-706E0D0EB6A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="5250" windowWidth="29040" windowHeight="15840" xr2:uid="{1E67AEA0-4F93-4754-A208-02BB9CB25A4A}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{1E67AEA0-4F93-4754-A208-02BB9CB25A4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -91,13 +91,15 @@
 As a consequence, cv.elw instruction is not covered</t>
   </si>
   <si>
-    <t>RTL freeze criteria for Dolphin Design but not for OpenHW Group. FSM Transition and State are encompassed by Branch, Condition and Statements code coverage.</t>
-  </si>
-  <si>
     <t xml:space="preserve">RTL freeze criteria for Dolphin Design but not for OpenHW Group.
 waived accordingly as considered not relevant
 not collected in simulation to save on performance
 </t>
+  </si>
+  <si>
+    <t>RTL freeze criteria for Dolphin Design but not for OpenHW Group.
+FSM Transition and State are encompassed by Branch, Condition and Statements code coverage.
+But this doesn't allow to catch Unreachable States and Unreacheable Transitions.</t>
   </si>
 </sst>
 </file>
@@ -244,18 +246,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -270,7 +269,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -287,6 +286,23 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -315,6 +331,21 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -342,6 +373,29 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -362,57 +416,26 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -443,6 +466,30 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -470,25 +517,26 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
           <color indexed="64"/>
         </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -510,55 +558,6 @@
       </font>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -573,27 +572,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9FB379CF-1833-48DB-8BB1-75AB0CF4E89C}" name="Tableau1" displayName="Tableau1" ref="B3:C7" headerRowCount="0" headerRowDxfId="11" headerRowBorderDxfId="14" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9FB379CF-1833-48DB-8BB1-75AB0CF4E89C}" name="Tableau1" displayName="Tableau1" ref="B3:C7" headerRowCount="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{664C0F73-DE64-4F2B-A49E-1DAFB3907496}" name="V1 identified holes still present in V2" totalsRowLabel="Total" headerRowDxfId="7" dataDxfId="13" totalsRowDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{A4B366C6-130B-441E-B6EF-8D4883947461}" name="Colonne1" totalsRowFunction="count" headerRowDxfId="8" dataDxfId="12" totalsRowDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{664C0F73-DE64-4F2B-A49E-1DAFB3907496}" name="V1 identified holes still present in V2" totalsRowLabel="Total" headerRowDxfId="12" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{A4B366C6-130B-441E-B6EF-8D4883947461}" name="Colonne1" totalsRowFunction="count" headerRowDxfId="9" dataDxfId="8" totalsRowDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{FE945D66-8D0A-4A00-B33D-E0F404A953E2}" name="Tableau4" displayName="Tableau4" ref="E3:F7" headerRowCount="0" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="5" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{FE945D66-8D0A-4A00-B33D-E0F404A953E2}" name="Tableau4" displayName="Tableau4" ref="E3:F7" headerRowCount="0" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{51D84596-7179-45C0-9516-1DEEF54FAEF1}" name="V2 holes " headerRowDxfId="0" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{4777E2C0-2819-4F1E-964F-A2D27E5B378B}" name="Colonne1" headerRowDxfId="1" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{51D84596-7179-45C0-9516-1DEEF54FAEF1}" name="V2 holes " headerRowDxfId="3" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{4777E2C0-2819-4F1E-964F-A2D27E5B378B}" name="Colonne1" headerRowDxfId="1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -912,99 +911,99 @@
   <dimension ref="B1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1"/>
-    <col min="2" max="2" width="57.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" style="1"/>
+    <col min="2" max="2" width="57.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="39" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="71" style="1" customWidth="1"/>
     <col min="6" max="6" width="42" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="1"/>
+    <col min="7" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
+    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="11" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="12"/>
+      <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+    <row r="6" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="E6" s="7" t="s">
+      <c r="C6" s="5"/>
+      <c r="E6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>